<commit_message>
Updated github Repo link to excel sheet
</commit_message>
<xml_diff>
--- a/Task1-4.xlsx
+++ b/Task1-4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fur4l\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fur4l\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4365366B-193C-4CB3-9FF9-9A4F6467C64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F940F2F-EB06-450A-894D-B7863219D6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{C4DA3F4E-C0FC-4087-8551-2D15F51B5CF3}"/>
+    <workbookView xWindow="348" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{C4DA3F4E-C0FC-4087-8551-2D15F51B5CF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>Next Character in Expression</t>
   </si>
@@ -192,16 +192,30 @@
   </si>
   <si>
     <t>Bottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github Repo: </t>
+  </si>
+  <si>
+    <t>https://github.com/Gary-Fox/Calc-o-stack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,14 +238,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -564,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F67DE68-299E-4430-8964-A52A6C8E480E}">
-  <dimension ref="A1:AC34"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,12 +981,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>49</v>
       </c>
@@ -981,7 +998,18 @@
         <v>33</v>
       </c>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C37" r:id="rId1" xr:uid="{48D6710D-B0F3-4A80-A98B-2539D2DD15BE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>